<commit_message>
Issue#30  Req 5.5  add main method for happy path  fix PreferDevManThatIsOlderThan30YearsOldStrategy VotingStrategy  calculation was wrong due to dividing by lower number then 30 years old  which is boundary from which we start to support such match
</commit_message>
<xml_diff>
--- a/Sample_SAP_DevMan_main_SAMPLE.xlsx
+++ b/Sample_SAP_DevMan_main_SAMPLE.xlsx
@@ -33,9 +33,6 @@
     <t>Initials</t>
   </si>
   <si>
-    <t>Employee Subgroup</t>
-  </si>
-  <si>
     <t>Job</t>
   </si>
   <si>
@@ -472,6 +469,9 @@
   </si>
   <si>
     <t>Poznan</t>
+  </si>
+  <si>
+    <t>Employee SubGroup</t>
   </si>
 </sst>
 </file>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.375" defaultRowHeight="12.45" x14ac:dyDescent="0.2"/>
@@ -1353,180 +1353,180 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>145</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="I2" s="5">
         <v>41764</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="7">
         <v>33442</v>
       </c>
       <c r="M2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="I3" s="5">
         <v>39295</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L3" s="7">
         <v>33443</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I4" s="5">
         <v>39342</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L4" s="7">
         <v>33444</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I5" s="5">
         <v>39342</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L5" s="7">
         <v>33445</v>
@@ -1534,31 +1534,31 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I6" s="5">
         <v>39388</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L6" s="7">
         <v>33446</v>
@@ -1566,31 +1566,31 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I7" s="5">
         <v>39433</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" s="7">
         <v>33447</v>
@@ -1598,29 +1598,29 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I8" s="5"/>
       <c r="J8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L8" s="7">
         <v>33448</v>
@@ -1628,29 +1628,29 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L9" s="7">
         <v>36737</v>
@@ -1658,29 +1658,29 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L10" s="7">
         <v>33450</v>
@@ -1688,26 +1688,26 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L11" s="7">
         <v>33451</v>
@@ -1715,23 +1715,23 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="L12" s="7">
         <v>33452</v>
@@ -1739,23 +1739,23 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L13" s="7">
         <v>33453</v>
@@ -1763,23 +1763,23 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" s="5"/>
       <c r="J14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L14" s="7">
         <v>33454</v>
@@ -1787,23 +1787,23 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L15" s="7">
         <v>33455</v>
@@ -1811,23 +1811,23 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" s="5"/>
       <c r="J16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L16" s="7">
         <v>33456</v>
@@ -1835,23 +1835,23 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I17" s="5"/>
       <c r="J17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L17" s="7">
         <v>33457</v>
@@ -1859,23 +1859,23 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I18" s="5"/>
       <c r="J18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L18" s="7">
         <v>33458</v>
@@ -1883,23 +1883,23 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I19" s="5"/>
       <c r="J19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L19" s="7">
         <v>33459</v>
@@ -1907,23 +1907,23 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I20" s="5"/>
       <c r="J20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K20" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L20" s="7">
         <v>33460</v>
@@ -1931,23 +1931,23 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I21" s="5"/>
       <c r="J21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L21" s="7">
         <v>33461</v>
@@ -1955,23 +1955,23 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="I22" s="5"/>
       <c r="J22" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K22" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="L22" s="7">
         <v>33462</v>
@@ -1979,23 +1979,23 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K23" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L23" s="7">
         <v>33463</v>
@@ -2003,23 +2003,23 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L24" s="7">
         <v>33464</v>
@@ -2027,23 +2027,23 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K25" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L25" s="7">
         <v>33465</v>
@@ -2051,20 +2051,20 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I26" s="5"/>
       <c r="J26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K26" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="L26" s="7">
         <v>33466</v>

</xml_diff>